<commit_message>
Added stop mark sensor Flowchart
</commit_message>
<xml_diff>
--- a/02Others/LogBook.xlsx
+++ b/02Others/LogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02Sem\LPI\DWR-19\02Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDD9AE5-2329-4E0D-AE07-EF32EDCA7F03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9A4510-C91B-4C8E-B85D-7B3CE41DA11A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTable" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
   <si>
     <t>Day</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Team Stats</t>
+  </si>
+  <si>
+    <t>Diagrama geral do sistema. Deteção de quartos.</t>
+  </si>
+  <si>
+    <t>https://www.eztronics.nl/webshop2/catalog/Sensor/Distance-Range?product_id=598</t>
   </si>
 </sst>
 </file>
@@ -301,14 +307,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,6 +328,61 @@
   </cellStyles>
   <dxfs count="39">
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -329,6 +390,34 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -336,6 +425,34 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -343,150 +460,39 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -502,14 +508,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{089AB311-2EBA-4666-A45A-92B70D0BB74D}" name="Tabela1" displayName="Tabela1" ref="A1:E24" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{089AB311-2EBA-4666-A45A-92B70D0BB74D}" name="Tabela1" displayName="Tabela1" ref="A1:E24" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A1:E24" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5AD32248-1077-464B-A7D3-70E7C7D94823}" name="Day" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{1C9ADB5E-D81F-498C-9278-7858E935AA74}" name="Start Time" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{ED087065-3F1F-4D46-914E-DD7DE82F29BC}" name="Tasks" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{93C97E1E-2A55-43A9-B68E-0598C0D09F28}" name="End Time" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{8EF2F89D-4902-4239-8ABF-0BE7E4EB90FB}" name="Duration" dataDxfId="32">
+    <tableColumn id="1" xr3:uid="{5AD32248-1077-464B-A7D3-70E7C7D94823}" name="Day" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{1C9ADB5E-D81F-498C-9278-7858E935AA74}" name="Start Time" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{ED087065-3F1F-4D46-914E-DD7DE82F29BC}" name="Tasks" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{93C97E1E-2A55-43A9-B68E-0598C0D09F28}" name="End Time" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{8EF2F89D-4902-4239-8ABF-0BE7E4EB90FB}" name="Duration" dataDxfId="31">
       <calculatedColumnFormula>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -518,14 +524,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DD9F9E8-D2B0-440B-927E-81876E34B61D}" name="Tabela14" displayName="Tabela14" ref="A1:E24" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DD9F9E8-D2B0-440B-927E-81876E34B61D}" name="Tabela14" displayName="Tabela14" ref="A1:E24" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A1:E24" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{85BD1EC3-C0E7-4EF0-98EF-4F01B8EAE2F3}" name="Day" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{80C27C96-FD1C-4830-8F54-DE84DCED9808}" name="Start Time" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{E682CF64-62B3-4421-B8AD-391788F8B766}" name="Tasks" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{55984218-71D5-4765-A54E-70BE13A4FCD0}" name="End Time" dataDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{43527839-801E-4BC5-98C8-9C34FFF7BB0E}" name="Duration" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{85BD1EC3-C0E7-4EF0-98EF-4F01B8EAE2F3}" name="Day" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{80C27C96-FD1C-4830-8F54-DE84DCED9808}" name="Start Time" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{E682CF64-62B3-4421-B8AD-391788F8B766}" name="Tasks" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{55984218-71D5-4765-A54E-70BE13A4FCD0}" name="End Time" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{43527839-801E-4BC5-98C8-9C34FFF7BB0E}" name="Duration" dataDxfId="23">
       <calculatedColumnFormula>Tabela14[[#This Row],[End Time]]-Tabela14[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -534,14 +540,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4CCCDC0E-C7E3-47B9-8789-B91B091ADD8C}" name="Tabela147" displayName="Tabela147" ref="A1:E24" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4CCCDC0E-C7E3-47B9-8789-B91B091ADD8C}" name="Tabela147" displayName="Tabela147" ref="A1:E24" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:E24" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A4DFB97C-4464-453F-AD2D-952EA90CBC4C}" name="Day" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{7359B1B8-25A1-488F-9454-F129E3980E2C}" name="Start Time" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{DB5689D0-C83B-4C58-97ED-3DC5F0173095}" name="Tasks" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{88D3CCB8-C055-417E-8841-9F5313B61FD7}" name="End Time" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{41FB43E1-33AF-4967-9F0E-5C323F87396C}" name="Duration" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{A4DFB97C-4464-453F-AD2D-952EA90CBC4C}" name="Day" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{7359B1B8-25A1-488F-9454-F129E3980E2C}" name="Start Time" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{DB5689D0-C83B-4C58-97ED-3DC5F0173095}" name="Tasks" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{88D3CCB8-C055-417E-8841-9F5313B61FD7}" name="End Time" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{41FB43E1-33AF-4967-9F0E-5C323F87396C}" name="Duration" dataDxfId="15">
       <calculatedColumnFormula>Tabela147[[#This Row],[End Time]]-Tabela147[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -550,14 +556,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F03DE230-AE05-4C03-AB82-A97CB3BB0939}" name="Tabela1478" displayName="Tabela1478" ref="A1:E24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F03DE230-AE05-4C03-AB82-A97CB3BB0939}" name="Tabela1478" displayName="Tabela1478" ref="A1:E24" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="A1:E24" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A3058E71-0408-4675-905B-61C9BCB4A03A}" name="Day" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{73EE3472-34B0-4B87-B603-EB02C7ACF80C}" name="Start Time" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{AB750483-1219-4286-A895-D20CC8A604A9}" name="Tasks" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{CDD8475B-DB00-4CBB-96E5-BC585B3E0DA4}" name="End Time" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{D80CBB36-36CA-48CD-A047-EB01578B76D2}" name="Duration" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{A3058E71-0408-4675-905B-61C9BCB4A03A}" name="Day" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{73EE3472-34B0-4B87-B603-EB02C7ACF80C}" name="Start Time" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{AB750483-1219-4286-A895-D20CC8A604A9}" name="Tasks" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CDD8475B-DB00-4CBB-96E5-BC585B3E0DA4}" name="End Time" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{D80CBB36-36CA-48CD-A047-EB01578B76D2}" name="Duration" dataDxfId="7">
       <calculatedColumnFormula>Tabela1478[[#This Row],[End Time]]-Tabela1478[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -566,14 +572,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E77EB429-0C66-46C5-A399-F393A25355E6}" name="Tabela2" displayName="Tabela2" ref="A5:E13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E77EB429-0C66-46C5-A399-F393A25355E6}" name="Tabela2" displayName="Tabela2" ref="A5:E13" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A5:E13" xr:uid="{911E91EB-1FF0-4A89-BC68-6C79F4F7C5B8}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{A529EA0B-F631-485F-93E8-036470D20E27}" name="Loja" dataDxfId="8"/>
-    <tableColumn id="1" xr3:uid="{EDF7F017-6B30-4C05-AB54-2B6FFD1E3BD0}" name="Produto" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{680017A8-58D2-4CFC-9B77-D751A4F9C07C}" name="QTD" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{F1F1EEB3-3097-4AE2-9314-8060F10DBFCF}" name="Preço_uni" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{CF896882-81A8-489C-B959-4EC89B14AAB9}" name="HiperLink" dataDxfId="4">
+    <tableColumn id="4" xr3:uid="{A529EA0B-F631-485F-93E8-036470D20E27}" name="Loja" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{EDF7F017-6B30-4C05-AB54-2B6FFD1E3BD0}" name="Produto" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{680017A8-58D2-4CFC-9B77-D751A4F9C07C}" name="QTD" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F1F1EEB3-3097-4AE2-9314-8060F10DBFCF}" name="Preço_uni" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CF896882-81A8-489C-B959-4EC89B14AAB9}" name="HiperLink" dataDxfId="0">
       <calculatedColumnFormula>HYPERLINK(,Tabela2[[#This Row],[Produto]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -880,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE379889-CFF8-440E-B1CF-7779A89E722A}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,10 +917,10 @@
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
@@ -933,7 +939,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>7.6388888888888951E-2</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="17" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="2">
@@ -957,7 +963,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>0</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="2">
@@ -981,7 +987,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>9.375E-2</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="2">
@@ -1023,10 +1029,10 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="17"/>
+      <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1045,7 +1051,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>8.3333333333333259E-2</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>29</v>
       </c>
       <c r="H7" s="13">
@@ -1070,7 +1076,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>9.0277777777777679E-2</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>5</v>
       </c>
       <c r="H8" s="14">
@@ -1115,10 +1121,10 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>0.10416666666666663</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="17"/>
+      <c r="H10" s="19"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1137,7 +1143,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>9.9999999999999978E-2</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="17" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="14">
@@ -1162,7 +1168,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>2.083333333333337E-2</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="17" t="s">
         <v>33</v>
       </c>
       <c r="H12" s="14">
@@ -1187,7 +1193,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>0.11458333333333331</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="17" t="s">
         <v>34</v>
       </c>
       <c r="H13" s="14">
@@ -1212,7 +1218,7 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>2.777777777777779E-2</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="17" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="14">
@@ -1237,12 +1243,12 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>6.25E-2</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="17" t="s">
         <v>36</v>
       </c>
       <c r="H15" s="14">
         <f>$H$8 + TimeTable_Team3!H3</f>
-        <v>1.103472222222222</v>
+        <v>0.22847222222222197</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1262,12 +1268,12 @@
         <f>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</f>
         <v>0.11458333333333326</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="17" t="s">
         <v>37</v>
       </c>
       <c r="H16" s="14">
         <f>$H$8 + TimeTable_Team3!H3</f>
-        <v>1.103472222222222</v>
+        <v>0.22847222222222197</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1377,7 +1383,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="A1:A24">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A20">
     <cfRule type="duplicateValues" priority="1"/>
@@ -1425,10 +1431,10 @@
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1483,10 +1489,10 @@
         <f>Tabela14[[#This Row],[End Time]]-Tabela14[[#This Row],[Start Time]]</f>
         <v>0</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -1694,7 +1700,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A24">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A20">
     <cfRule type="duplicateValues" priority="1"/>
@@ -1742,10 +1748,10 @@
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -1800,10 +1806,10 @@
         <f>Tabela147[[#This Row],[End Time]]-Tabela147[[#This Row],[Start Time]]</f>
         <v>0</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -2011,7 +2017,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A24">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A20">
     <cfRule type="duplicateValues" priority="1"/>
@@ -2029,7 +2035,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2059,26 +2065,32 @@
       <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="17"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="A2" s="2">
+        <v>44286</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3">
         <f>Tabela1478[[#This Row],[End Time]]-Tabela1478[[#This Row],[Start Time]]</f>
-        <v>0</v>
+        <v>-0.875</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="13">
         <f>COUNT(Tabela1478[[#All],[Day]])</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2095,7 +2107,7 @@
       </c>
       <c r="H3" s="14">
         <f>SUM(Tabela1478[[#All],[Duration]])</f>
-        <v>0</v>
+        <v>-0.875</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2117,10 +2129,10 @@
         <f>Tabela1478[[#This Row],[End Time]]-Tabela1478[[#This Row],[Start Time]]</f>
         <v>0</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="17"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -2328,7 +2340,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A24">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A20">
     <cfRule type="duplicateValues" priority="1"/>
@@ -2343,10 +2355,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C227607-00A4-48AA-9A87-27CE805F8079}">
-  <dimension ref="A2:E13"/>
+  <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2508,6 +2520,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added obstacles sensor flowchart
</commit_message>
<xml_diff>
--- a/02Others/LogBook.xlsx
+++ b/02Others/LogBook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02Sem\LPI\DWR-19\02Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9A4510-C91B-4C8E-B85D-7B3CE41DA11A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1977F368-CD74-42D4-8B8C-708120A6384D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTable" sheetId="1" r:id="rId1"/>
@@ -166,10 +166,10 @@
     <t>Team Stats</t>
   </si>
   <si>
-    <t>Diagrama geral do sistema. Deteção de quartos.</t>
-  </si>
-  <si>
     <t>https://www.eztronics.nl/webshop2/catalog/Sensor/Distance-Range?product_id=598</t>
+  </si>
+  <si>
+    <t>Diagrama geral do sistema. Deteção de quartos e cruzamentos.</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1248,7 @@
       </c>
       <c r="H15" s="14">
         <f>$H$8 + TimeTable_Team3!H3</f>
-        <v>0.22847222222222197</v>
+        <v>1.2145833333333331</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="H16" s="14">
         <f>$H$8 + TimeTable_Team3!H3</f>
-        <v>0.22847222222222197</v>
+        <v>1.2145833333333331</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2034,8 +2034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB61F12-31A1-4865-A365-EE2C93760A20}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2078,12 +2078,14 @@
         <v>0.875</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>43</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.98611111111111116</v>
+      </c>
       <c r="E2" s="3">
         <f>Tabela1478[[#This Row],[End Time]]-Tabela1478[[#This Row],[Start Time]]</f>
-        <v>-0.875</v>
+        <v>0.11111111111111116</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>29</v>
@@ -2107,7 +2109,7 @@
       </c>
       <c r="H3" s="14">
         <f>SUM(Tabela1478[[#All],[Duration]])</f>
-        <v>-0.875</v>
+        <v>0.11111111111111116</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2357,7 +2359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C227607-00A4-48AA-9A87-27CE805F8079}">
   <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2522,7 +2524,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Joao/Duarte update logbook -> day 31/03
</commit_message>
<xml_diff>
--- a/02Others/LogBook.xlsx
+++ b/02Others/LogBook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02Sem\LPI\DWR-19\02Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoaoMiranda\Desktop\ProjetosUM\DWR-19\02Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1977F368-CD74-42D4-8B8C-708120A6384D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55B17CE-0939-41BB-9AA5-8BB295F85126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTable" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>Day</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>Diagrama geral do sistema. Deteção de quartos e cruzamentos.</t>
+  </si>
+  <si>
+    <t>Estudo do seguidor de linha. Uso do DMA para ler 2 inputs do sensor</t>
   </si>
 </sst>
 </file>
@@ -890,18 +893,18 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -922,7 +925,7 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44253</v>
       </c>
@@ -946,7 +949,7 @@
         <v>44260</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44258</v>
       </c>
@@ -970,7 +973,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44263</v>
       </c>
@@ -994,7 +997,7 @@
         <v>44370</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44263</v>
       </c>
@@ -1012,7 +1015,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44265</v>
       </c>
@@ -1034,7 +1037,7 @@
       </c>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44270</v>
       </c>
@@ -1059,7 +1062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44272</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>1.103472222222222</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44273</v>
       </c>
@@ -1104,7 +1107,7 @@
       <c r="G9" s="14"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44277</v>
       </c>
@@ -1126,7 +1129,7 @@
       </c>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44277</v>
       </c>
@@ -1148,10 +1151,10 @@
       </c>
       <c r="H11" s="14">
         <f>$H$8 + TimeTable_Team1!H3</f>
-        <v>1.103472222222222</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.3256944444444441</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44278</v>
       </c>
@@ -1173,10 +1176,10 @@
       </c>
       <c r="H12" s="14">
         <f>$H$8 + TimeTable_Team1!H3</f>
-        <v>1.103472222222222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1.3256944444444441</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44279</v>
       </c>
@@ -1201,7 +1204,7 @@
         <v>1.103472222222222</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44279</v>
       </c>
@@ -1226,7 +1229,7 @@
         <v>1.103472222222222</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44279</v>
       </c>
@@ -1251,7 +1254,7 @@
         <v>1.2145833333333331</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44279</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>1.2145833333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44280</v>
       </c>
@@ -1295,7 +1298,7 @@
       </c>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44281</v>
       </c>
@@ -1314,7 +1317,7 @@
       </c>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1325,7 +1328,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1335,7 +1338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1345,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1355,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1365,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1400,22 +1403,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2A9EC5-EFB6-4F84-81FA-9F8B291BBBD8}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1436,24 +1439,32 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>44286</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.80555555555555547</v>
+      </c>
       <c r="E2" s="3">
         <f>Tabela14[[#This Row],[End Time]]-Tabela14[[#This Row],[Start Time]]</f>
-        <v>0</v>
+        <v>0.2222222222222221</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="13">
         <f>COUNT(Tabela14[[#All],[Day]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1467,10 +1478,10 @@
       </c>
       <c r="H3" s="14">
         <f>SUM(Tabela14[[#All],[Duration]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2222222222222221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1480,7 +1491,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -1494,7 +1505,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -1508,7 +1519,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1522,7 +1533,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -1532,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1542,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1552,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1562,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1572,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1582,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1592,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1602,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1612,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1622,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1632,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1642,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1652,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1662,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1672,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1682,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1721,18 +1732,18 @@
       <selection activeCell="G1" sqref="G1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1753,7 +1764,7 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="4"/>
@@ -1770,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1787,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1797,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -1811,7 +1822,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -1825,7 +1836,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1839,7 +1850,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -1849,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1859,7 +1870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1869,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1879,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1889,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1899,7 +1910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1909,7 +1920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1919,7 +1930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1929,7 +1940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1939,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1949,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1959,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1969,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1979,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1989,7 +2000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1999,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2034,22 +2045,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB61F12-31A1-4865-A365-EE2C93760A20}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +2081,7 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44286</v>
       </c>
@@ -2095,7 +2106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -2112,7 +2123,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -2122,7 +2133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -2136,7 +2147,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -2150,7 +2161,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -2164,7 +2175,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -2174,7 +2185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -2184,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -2194,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -2204,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -2214,7 +2225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -2224,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -2234,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -2244,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -2254,7 +2265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -2264,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -2274,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -2284,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -2294,7 +2305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -2304,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -2314,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -2324,7 +2335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2363,16 +2374,16 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="55.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="55.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
@@ -2381,7 +2392,7 @@
         <v>37.770000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -2398,7 +2409,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
@@ -2416,7 +2427,7 @@
         <v>Bluetooth Module HC-05</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -2434,7 +2445,7 @@
         <v>IR Emitter and Receiver LED 5mm 940nm</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -2452,7 +2463,7 @@
         <v>OV7670 Camera Module</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
@@ -2470,7 +2481,7 @@
         <v>TCS3200 Color Sensor</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
@@ -2488,7 +2499,7 @@
         <v>US-015 Modulo Sensor de Distância Ultrassónico 3.3 - 5V</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="1">
@@ -2502,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="1"/>
@@ -2512,7 +2523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="1"/>
@@ -2522,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Added RFID code, Updated logbook and components list
</commit_message>
<xml_diff>
--- a/02Others/LogBook.xlsx
+++ b/02Others/LogBook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoaoMiranda\Desktop\ProjetosUM\DWR-19\02Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/a88231_uminho_pt/Documents/Universidade/Github/dwr-19/02Others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55B17CE-0939-41BB-9AA5-8BB295F85126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{F55B17CE-0939-41BB-9AA5-8BB295F85126}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D65F682B-4F48-49D7-9E7D-ED5C6148F979}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTable" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t>Day</t>
   </si>
@@ -173,6 +173,15 @@
   </si>
   <si>
     <t>Estudo do seguidor de linha. Uso do DMA para ler 2 inputs do sensor</t>
+  </si>
+  <si>
+    <t>Criação do modulo para a leitura de etiquetas RFID</t>
+  </si>
+  <si>
+    <t>MAUSER</t>
+  </si>
+  <si>
+    <t>Módulo Leitor RFID RC522</t>
   </si>
 </sst>
 </file>
@@ -262,7 +271,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -322,6 +331,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Cor1" xfId="1" builtinId="29"/>
@@ -893,18 +903,18 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -925,7 +935,7 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44253</v>
       </c>
@@ -949,7 +959,7 @@
         <v>44260</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44258</v>
       </c>
@@ -973,7 +983,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44263</v>
       </c>
@@ -997,7 +1007,7 @@
         <v>44370</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44263</v>
       </c>
@@ -1015,7 +1025,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44265</v>
       </c>
@@ -1037,7 +1047,7 @@
       </c>
       <c r="H6" s="19"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44270</v>
       </c>
@@ -1062,7 +1072,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44272</v>
       </c>
@@ -1087,7 +1097,7 @@
         <v>1.103472222222222</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44273</v>
       </c>
@@ -1107,7 +1117,7 @@
       <c r="G9" s="14"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44277</v>
       </c>
@@ -1129,7 +1139,7 @@
       </c>
       <c r="H10" s="19"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44277</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>1.3256944444444441</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44278</v>
       </c>
@@ -1179,7 +1189,7 @@
         <v>1.3256944444444441</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44279</v>
       </c>
@@ -1201,10 +1211,10 @@
       </c>
       <c r="H13" s="14">
         <f>$H$8 + TimeTable_Team2!H3</f>
-        <v>1.103472222222222</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.3048611111111108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44279</v>
       </c>
@@ -1226,10 +1236,10 @@
       </c>
       <c r="H14" s="14">
         <f>$H$8 + TimeTable_Team2!H3</f>
-        <v>1.103472222222222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.3048611111111108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44279</v>
       </c>
@@ -1254,7 +1264,7 @@
         <v>1.2145833333333331</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44279</v>
       </c>
@@ -1279,7 +1289,7 @@
         <v>1.2145833333333331</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44280</v>
       </c>
@@ -1298,7 +1308,7 @@
       </c>
       <c r="H17"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44281</v>
       </c>
@@ -1317,7 +1327,7 @@
       </c>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1328,7 +1338,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1338,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1348,7 +1358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1358,7 +1368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1368,7 +1378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1403,22 +1413,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A2A9EC5-EFB6-4F84-81FA-9F8B291BBBD8}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1449,7 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44286</v>
       </c>
@@ -1464,7 +1474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1481,7 +1491,7 @@
         <v>0.2222222222222221</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1491,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -1505,7 +1515,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -1519,7 +1529,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1533,7 +1543,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -1543,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1553,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1563,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1573,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1583,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1593,7 +1603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1603,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1613,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1623,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1633,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1643,7 +1653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1653,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1663,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1673,7 +1683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -1683,7 +1693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -1693,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -1728,22 +1738,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F1DF70-9EAC-49DC-AC3E-822A07B27930}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1764,24 +1774,32 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44300</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.97222222222222221</v>
+      </c>
       <c r="E2" s="3">
         <f>Tabela147[[#This Row],[End Time]]-Tabela147[[#This Row],[Start Time]]</f>
-        <v>0</v>
+        <v>0.20138888888888884</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="13">
         <f>COUNT(Tabela147[[#All],[Day]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -1795,10 +1813,10 @@
       </c>
       <c r="H3" s="14">
         <f>SUM(Tabela147[[#All],[Duration]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.20138888888888884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -1808,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -1822,7 +1840,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -1836,7 +1854,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -1850,7 +1868,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -1860,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -1870,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -1880,7 +1898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -1890,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -1900,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -1910,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -1920,7 +1938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -1930,7 +1948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -1940,7 +1958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -1950,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -1960,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -1970,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -1980,7 +1998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -1990,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -2000,7 +2018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -2010,7 +2028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2046,21 +2064,21 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2081,7 +2099,7 @@
       </c>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44286</v>
       </c>
@@ -2106,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="4"/>
@@ -2123,7 +2141,7 @@
         <v>0.11111111111111116</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4"/>
@@ -2133,7 +2151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
@@ -2147,7 +2165,7 @@
       </c>
       <c r="H5" s="19"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -2161,7 +2179,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -2175,7 +2193,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -2185,7 +2203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -2195,7 +2213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -2205,7 +2223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -2215,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -2225,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -2235,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -2245,7 +2263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -2255,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -2265,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -2275,7 +2293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -2285,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -2295,7 +2313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -2305,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -2315,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -2325,7 +2343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -2335,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2370,29 +2388,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C227607-00A4-48AA-9A87-27CE805F8079}">
   <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="55.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="55.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="51.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="7">
         <f>SUMPRODUCT(Tabela2[QTD], Tabela2[Preço_uni])</f>
-        <v>37.770000000000003</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40.21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -2409,7 +2427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
@@ -2427,7 +2445,7 @@
         <v>Bluetooth Module HC-05</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -2445,7 +2463,7 @@
         <v>IR Emitter and Receiver LED 5mm 940nm</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
@@ -2463,7 +2481,7 @@
         <v>OV7670 Camera Module</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>13</v>
       </c>
@@ -2481,7 +2499,7 @@
         <v>TCS3200 Color Sensor</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
@@ -2499,21 +2517,25 @@
         <v>US-015 Modulo Sensor de Distância Ultrassónico 3.3 - 5V</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="C11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="8">
-        <v>0</v>
-      </c>
-      <c r="E11" s="9">
-        <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.44</v>
+      </c>
+      <c r="E11" s="9" t="str">
+        <f>HYPERLINK("https://mauser.pt/catalog/product_info.php?cPath=1667_2604_2607&amp;products_id=096-8517",Tabela2[[#This Row],[Produto]])</f>
+        <v>Módulo Leitor RFID RC522</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="1"/>
@@ -2523,7 +2545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="1"/>
@@ -2533,16 +2555,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B15" r:id="rId1" xr:uid="{3BE2CB3D-1045-4FA3-95C3-6C6F5D5C6679}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Logbook and added Perifericos
</commit_message>
<xml_diff>
--- a/02Others/LogBook.xlsx
+++ b/02Others/LogBook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\DWR-19\02Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/a88231_uminho_pt/Documents/Documentos/Github/DWR-19/02Others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43D4005-673E-4E45-AE84-8EF99CB0CD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{F43D4005-673E-4E45-AE84-8EF99CB0CD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97BD2AC5-BA65-4CB7-B263-719F87F6F790}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTable" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
   <si>
     <t>Day</t>
   </si>
@@ -190,9 +190,6 @@
     <t>Implementação da deteção de obstáculos, quartos e cruzamentos.</t>
   </si>
   <si>
-    <t>estudo do modulo RFID</t>
-  </si>
-  <si>
     <t>Continuação da implementação do modulo RFID + documentação</t>
   </si>
   <si>
@@ -260,6 +257,12 @@
   </si>
   <si>
     <t>Montagem Robô</t>
+  </si>
+  <si>
+    <t>Estudo e Implementação do Bluetooth</t>
+  </si>
+  <si>
+    <t>Estudo do modulo RFID</t>
   </si>
 </sst>
 </file>
@@ -378,7 +381,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -468,6 +471,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1050,8 +1062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE379889-CFF8-440E-B1CF-7779A89E722A}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1417,7 @@
       </c>
       <c r="H15" s="12">
         <f>$H$10 + TimeTable_Team2!H3</f>
-        <v>1.9229166666666666</v>
+        <v>2.0895833333333336</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1430,7 +1442,7 @@
       </c>
       <c r="H16" s="12">
         <f>$H$10 + TimeTable_Team2!H3</f>
-        <v>1.9229166666666666</v>
+        <v>2.0895833333333336</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1510,7 +1522,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="3">
         <v>0.70833333333333337</v>
@@ -1528,7 +1540,7 @@
         <v>0.875</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
@@ -1546,7 +1558,7 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="29">
         <v>0.83333333333333337</v>
@@ -1564,7 +1576,7 @@
         <v>0.60416666666666663</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="3">
         <v>0.70833333333333337</v>
@@ -1582,7 +1594,7 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D24" s="3">
         <v>0.55208333333333337</v>
@@ -1750,7 +1762,7 @@
         <v>0.375</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="3">
         <v>0.83333333333333337</v>
@@ -1775,7 +1787,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D4" s="3">
         <v>0.79166666666666663</v>
@@ -1793,7 +1805,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5" s="3">
         <v>0.77083333333333337</v>
@@ -2036,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F1DF70-9EAC-49DC-AC3E-822A07B27930}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2080,7 +2092,7 @@
         <v>0.85416666666666663</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="D2" s="3">
         <v>0.89583333333333337</v>
@@ -2094,7 +2106,7 @@
       </c>
       <c r="H2" s="11">
         <f>COUNT(Tabela147[[#All],[Day]])</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2119,7 +2131,7 @@
       </c>
       <c r="H3" s="12">
         <f>SUM(Tabela147[[#All],[Duration]])</f>
-        <v>0.40625</v>
+        <v>0.57291666666666674</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2130,7 +2142,7 @@
         <v>0.57638888888888895</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>0.73958333333333337</v>
@@ -2141,9 +2153,21 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="32">
+        <v>44352</v>
+      </c>
+      <c r="B5" s="33">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="E5" s="3">
         <f>Tabela147[[#This Row],[End Time]]-Tabela147[[#This Row],[Start Time]]</f>
-        <v>0</v>
+        <v>0.16666666666666674</v>
       </c>
       <c r="G5" s="30" t="s">
         <v>39</v>
@@ -2380,7 +2404,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,7 +2497,7 @@
         <v>0.375</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="3">
         <v>0.83333333333333337</v>
@@ -2869,10 +2893,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -2887,10 +2911,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -2905,10 +2929,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" s="1">
         <v>6</v>
@@ -2923,10 +2947,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1">
         <v>6</v>
@@ -2941,10 +2965,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -2960,10 +2984,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="1">
         <v>6</v>
@@ -2979,10 +3003,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -2998,10 +3022,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
@@ -3017,10 +3041,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
@@ -3036,10 +3060,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1">
         <v>1</v>
@@ -3055,10 +3079,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>68</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>69</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
atulizaçao do logbook | lista de componentes | ordem de trabalhos
</commit_message>
<xml_diff>
--- a/02Others/LogBook.xlsx
+++ b/02Others/LogBook.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\02Sem\LPI\DWR-19\02Others\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoaoMiranda\Desktop\ProjetosUM\DWR-19\02Others\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368142DF-6118-4871-8B04-1D0C3FCADA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C20CC8C-354A-4032-A21D-31610281C9C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="4" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{81FA8CF0-04E5-4214-83E0-2D0ED2A04D15}"/>
   </bookViews>
   <sheets>
     <sheet name="TimeTable" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Components" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="95">
   <si>
     <t>Day</t>
   </si>
@@ -281,6 +282,48 @@
   </si>
   <si>
     <t>Manga Espiral Wrapping 20-60mm</t>
+  </si>
+  <si>
+    <t>Fusivel 3A</t>
+  </si>
+  <si>
+    <t>Guimocircuito</t>
+  </si>
+  <si>
+    <t>PCB Shield STM32F767ZI</t>
+  </si>
+  <si>
+    <t>Mauser</t>
+  </si>
+  <si>
+    <t>Barra (2x8) fêmea 2,54 mm PCB</t>
+  </si>
+  <si>
+    <t>Barra (2x10) fêmea 2,54 mm PCB</t>
+  </si>
+  <si>
+    <t>Barra (2x16) fêmea 2,54 mm PCB</t>
+  </si>
+  <si>
+    <t>Barra (2x17) fêmea 2,54 mm PCB</t>
+  </si>
+  <si>
+    <t>Barra (2x3) fêmea 2,54 mm PCB</t>
+  </si>
+  <si>
+    <t>Barra (1x6) fêmea 2,54 mm PCB</t>
+  </si>
+  <si>
+    <t>Parte Mecânica (Sensor Distancia/Sensor linha/Furos Fonte/RFID)</t>
+  </si>
+  <si>
+    <t>Montagem integral dos circuitos (I)</t>
+  </si>
+  <si>
+    <t>Montagem integral dos circuitos (II)</t>
+  </si>
+  <si>
+    <t>Diagramas mecânicos</t>
   </si>
 </sst>
 </file>
@@ -510,62 +553,7 @@
     <cellStyle name="Hiperligação" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="45">
     <dxf>
       <fill>
         <patternFill>
@@ -574,34 +562,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -616,39 +576,150 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -706,14 +777,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{089AB311-2EBA-4666-A45A-92B70D0BB74D}" name="Tabela1" displayName="Tabela1" ref="A1:E40" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{089AB311-2EBA-4666-A45A-92B70D0BB74D}" name="Tabela1" displayName="Tabela1" ref="A1:E40" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:E40" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{5AD32248-1077-464B-A7D3-70E7C7D94823}" name="Day" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{1C9ADB5E-D81F-498C-9278-7858E935AA74}" name="Start Time" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{ED087065-3F1F-4D46-914E-DD7DE82F29BC}" name="Tasks" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{93C97E1E-2A55-43A9-B68E-0598C0D09F28}" name="End Time" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{8EF2F89D-4902-4239-8ABF-0BE7E4EB90FB}" name="Duration" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{5AD32248-1077-464B-A7D3-70E7C7D94823}" name="Day" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{1C9ADB5E-D81F-498C-9278-7858E935AA74}" name="Start Time" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{ED087065-3F1F-4D46-914E-DD7DE82F29BC}" name="Tasks" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{93C97E1E-2A55-43A9-B68E-0598C0D09F28}" name="End Time" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{8EF2F89D-4902-4239-8ABF-0BE7E4EB90FB}" name="Duration" dataDxfId="37">
       <calculatedColumnFormula>Tabela1[[#This Row],[End Time]]-Tabela1[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -722,14 +793,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DD9F9E8-D2B0-440B-927E-81876E34B61D}" name="Tabela14" displayName="Tabela14" ref="A1:E24" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{7DD9F9E8-D2B0-440B-927E-81876E34B61D}" name="Tabela14" displayName="Tabela14" ref="A1:E24" totalsRowShown="0" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:E24" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{85BD1EC3-C0E7-4EF0-98EF-4F01B8EAE2F3}" name="Day" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{80C27C96-FD1C-4830-8F54-DE84DCED9808}" name="Start Time" dataDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{E682CF64-62B3-4421-B8AD-391788F8B766}" name="Tasks" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{55984218-71D5-4765-A54E-70BE13A4FCD0}" name="End Time" dataDxfId="25"/>
-    <tableColumn id="6" xr3:uid="{43527839-801E-4BC5-98C8-9C34FFF7BB0E}" name="Duration" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{85BD1EC3-C0E7-4EF0-98EF-4F01B8EAE2F3}" name="Day" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{80C27C96-FD1C-4830-8F54-DE84DCED9808}" name="Start Time" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{E682CF64-62B3-4421-B8AD-391788F8B766}" name="Tasks" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{55984218-71D5-4765-A54E-70BE13A4FCD0}" name="End Time" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{43527839-801E-4BC5-98C8-9C34FFF7BB0E}" name="Duration" dataDxfId="29">
       <calculatedColumnFormula>Tabela14[[#This Row],[End Time]]-Tabela14[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -738,14 +809,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4CCCDC0E-C7E3-47B9-8789-B91B091ADD8C}" name="Tabela147" displayName="Tabela147" ref="A1:E24" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4CCCDC0E-C7E3-47B9-8789-B91B091ADD8C}" name="Tabela147" displayName="Tabela147" ref="A1:E24" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A1:E24" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A4DFB97C-4464-453F-AD2D-952EA90CBC4C}" name="Day" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{7359B1B8-25A1-488F-9454-F129E3980E2C}" name="Start Time" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{DB5689D0-C83B-4C58-97ED-3DC5F0173095}" name="Tasks" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{88D3CCB8-C055-417E-8841-9F5313B61FD7}" name="End Time" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{41FB43E1-33AF-4967-9F0E-5C323F87396C}" name="Duration" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{A4DFB97C-4464-453F-AD2D-952EA90CBC4C}" name="Day" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{7359B1B8-25A1-488F-9454-F129E3980E2C}" name="Start Time" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{DB5689D0-C83B-4C58-97ED-3DC5F0173095}" name="Tasks" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{88D3CCB8-C055-417E-8841-9F5313B61FD7}" name="End Time" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{41FB43E1-33AF-4967-9F0E-5C323F87396C}" name="Duration" dataDxfId="20">
       <calculatedColumnFormula>Tabela147[[#This Row],[End Time]]-Tabela147[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -754,14 +825,14 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F03DE230-AE05-4C03-AB82-A97CB3BB0939}" name="Tabela1478" displayName="Tabela1478" ref="A1:E24" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F03DE230-AE05-4C03-AB82-A97CB3BB0939}" name="Tabela1478" displayName="Tabela1478" ref="A1:E24" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:E24" xr:uid="{1B66A83B-1E9C-400A-A414-4BA5EB76EA0B}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A3058E71-0408-4675-905B-61C9BCB4A03A}" name="Day" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{73EE3472-34B0-4B87-B603-EB02C7ACF80C}" name="Start Time" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{AB750483-1219-4286-A895-D20CC8A604A9}" name="Tasks" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{CDD8475B-DB00-4CBB-96E5-BC585B3E0DA4}" name="End Time" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{D80CBB36-36CA-48CD-A047-EB01578B76D2}" name="Duration" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{A3058E71-0408-4675-905B-61C9BCB4A03A}" name="Day" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{73EE3472-34B0-4B87-B603-EB02C7ACF80C}" name="Start Time" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{AB750483-1219-4286-A895-D20CC8A604A9}" name="Tasks" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{CDD8475B-DB00-4CBB-96E5-BC585B3E0DA4}" name="End Time" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{D80CBB36-36CA-48CD-A047-EB01578B76D2}" name="Duration" dataDxfId="12">
       <calculatedColumnFormula>Tabela1478[[#This Row],[End Time]]-Tabela1478[[#This Row],[Start Time]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -770,14 +841,14 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E77EB429-0C66-46C5-A399-F393A25355E6}" name="Tabela2" displayName="Tabela2" ref="A5:E27" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A5:E27" xr:uid="{911E91EB-1FF0-4A89-BC68-6C79F4F7C5B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E77EB429-0C66-46C5-A399-F393A25355E6}" name="Tabela2" displayName="Tabela2" ref="A5:E34" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A5:E34" xr:uid="{911E91EB-1FF0-4A89-BC68-6C79F4F7C5B8}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{A529EA0B-F631-485F-93E8-036470D20E27}" name="Loja" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{EDF7F017-6B30-4C05-AB54-2B6FFD1E3BD0}" name="Produto" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{680017A8-58D2-4CFC-9B77-D751A4F9C07C}" name="QTD" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F1F1EEB3-3097-4AE2-9314-8060F10DBFCF}" name="Preço_uni" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CF896882-81A8-489C-B959-4EC89B14AAB9}" name="HiperLink" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{A529EA0B-F631-485F-93E8-036470D20E27}" name="Loja" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{EDF7F017-6B30-4C05-AB54-2B6FFD1E3BD0}" name="Produto" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{680017A8-58D2-4CFC-9B77-D751A4F9C07C}" name="QTD" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{F1F1EEB3-3097-4AE2-9314-8060F10DBFCF}" name="Preço_uni" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CF896882-81A8-489C-B959-4EC89B14AAB9}" name="HiperLink" dataDxfId="5">
       <calculatedColumnFormula>HYPERLINK(,Tabela2[[#This Row],[Produto]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1084,22 +1155,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE379889-CFF8-440E-B1CF-7779A89E722A}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="34" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" style="34" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1191,7 @@
       </c>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44253</v>
       </c>
@@ -1144,7 +1215,7 @@
         <v>44260</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44258</v>
       </c>
@@ -1168,7 +1239,7 @@
         <v>44281</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44263</v>
       </c>
@@ -1192,7 +1263,7 @@
         <v>44369</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44263</v>
       </c>
@@ -1210,7 +1281,7 @@
         <v>4.861111111111116E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>44265</v>
       </c>
@@ -1232,10 +1303,10 @@
       </c>
       <c r="H6" s="18">
         <f ca="1">_xlfn.DAYS(MAX(H2:H4), TODAY())</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>44270</v>
       </c>
@@ -1253,7 +1324,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>44272</v>
       </c>
@@ -1275,7 +1346,7 @@
       </c>
       <c r="H8" s="35"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>44273</v>
       </c>
@@ -1300,7 +1371,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>44277</v>
       </c>
@@ -1325,7 +1396,7 @@
         <v>4.7874999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>44277</v>
       </c>
@@ -1345,7 +1416,7 @@
       <c r="G11" s="12"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>44278</v>
       </c>
@@ -1367,7 +1438,7 @@
       </c>
       <c r="H12" s="35"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>44279</v>
       </c>
@@ -1389,10 +1460,10 @@
       </c>
       <c r="H13" s="12">
         <f>$H$10 + TimeTable_Team1!H3</f>
-        <v>5.780555555555555</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6.426388888888888</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>44279</v>
       </c>
@@ -1414,10 +1485,10 @@
       </c>
       <c r="H14" s="12">
         <f>$H$10 + TimeTable_Team1!H3</f>
-        <v>5.780555555555555</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>6.426388888888888</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>44279</v>
       </c>
@@ -1439,10 +1510,10 @@
       </c>
       <c r="H15" s="12">
         <f>$H$10 + TimeTable_Team2!H3</f>
-        <v>5.3604166666666666</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>5.4854166666666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>44279</v>
       </c>
@@ -1464,10 +1535,10 @@
       </c>
       <c r="H16" s="12">
         <f>$H$10 + TimeTable_Team2!H3</f>
-        <v>5.3604166666666666</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>5.4854166666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>44280</v>
       </c>
@@ -1492,7 +1563,7 @@
         <v>5.6451388888888889</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>44281</v>
       </c>
@@ -1517,7 +1588,7 @@
         <v>5.6451388888888889</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>44319</v>
       </c>
@@ -1536,7 +1607,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>44349</v>
       </c>
@@ -1554,7 +1625,7 @@
         <v>0.10416666666666674</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>44349</v>
       </c>
@@ -1572,7 +1643,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>44350</v>
       </c>
@@ -1590,7 +1661,7 @@
         <v>0.43750000000000006</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>44351</v>
       </c>
@@ -1608,7 +1679,7 @@
         <v>0.10416666666666674</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>44354</v>
       </c>
@@ -1626,7 +1697,7 @@
         <v>0.15625000000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>44354</v>
       </c>
@@ -1644,7 +1715,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>44355</v>
       </c>
@@ -1662,7 +1733,7 @@
         <v>0.60416666666666674</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>44356</v>
       </c>
@@ -1680,7 +1751,7 @@
         <v>4.1666666666666741E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>44356</v>
       </c>
@@ -1698,7 +1769,7 @@
         <v>0.58333333333333326</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>44356</v>
       </c>
@@ -1716,7 +1787,7 @@
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>44357</v>
       </c>
@@ -1734,7 +1805,7 @@
         <v>0.60416666666666674</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>44358</v>
       </c>
@@ -1752,7 +1823,7 @@
         <v>0.39583333333333337</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="4"/>
@@ -1762,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
       <c r="C33" s="4"/>
@@ -1772,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
       <c r="C34" s="4"/>
@@ -1782,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="3"/>
       <c r="C35" s="4"/>
@@ -1792,7 +1863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="3"/>
       <c r="C36" s="4"/>
@@ -1802,7 +1873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="3"/>
       <c r="C37" s="4"/>
@@ -1812,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="3"/>
       <c r="C38" s="4"/>
@@ -1822,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="3"/>
       <c r="C39" s="4"/>
@@ -1832,7 +1903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="3"/>
       <c r="C40" s="4"/>
@@ -1849,11 +1920,14 @@
     <mergeCell ref="G12:H12"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A40">
-    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
+  <conditionalFormatting sqref="A1:A31 A33:A40">
+    <cfRule type="duplicateValues" dxfId="44" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A20">
-    <cfRule type="duplicateValues" priority="1"/>
+    <cfRule type="duplicateValues" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1868,21 +1942,21 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="69" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1903,7 +1977,7 @@
       </c>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44286</v>
       </c>
@@ -1925,10 +1999,10 @@
       </c>
       <c r="H2" s="11">
         <f>COUNT(Tabela14[[#All],[Day]])</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44348</v>
       </c>
@@ -1950,10 +2024,10 @@
       </c>
       <c r="H3" s="12">
         <f>SUM(Tabela14[[#All],[Duration]])</f>
-        <v>0.99305555555555547</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>1.6388888888888884</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44352</v>
       </c>
@@ -1971,7 +2045,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44353</v>
       </c>
@@ -1993,45 +2067,69 @@
       </c>
       <c r="H5" s="35"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>44359</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.77083333333333337</v>
+      </c>
       <c r="E6" s="3">
         <f>Tabela14[[#This Row],[End Time]]-Tabela14[[#This Row],[Start Time]]</f>
-        <v>0</v>
+        <v>0.1875</v>
       </c>
       <c r="G6" s="36" t="s">
         <v>32</v>
       </c>
       <c r="H6" s="36"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44360</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.54166666666666663</v>
+      </c>
       <c r="E7" s="3">
         <f>Tabela14[[#This Row],[End Time]]-Tabela14[[#This Row],[Start Time]]</f>
-        <v>0</v>
+        <v>0.16666666666666663</v>
       </c>
       <c r="G7" s="36" t="s">
         <v>33</v>
       </c>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44360</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.875</v>
+      </c>
       <c r="E8" s="3">
         <f>Tabela14[[#This Row],[End Time]]-Tabela14[[#This Row],[Start Time]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.29166666666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -2041,7 +2139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -2051,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -2061,7 +2159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -2071,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -2081,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -2091,7 +2189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -2101,7 +2199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -2111,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -2121,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -2131,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -2141,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -2151,7 +2249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -2161,7 +2259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -2171,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -2181,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2198,16 +2296,22 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G1:H1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A1:A2 A4:A24">
-    <cfRule type="duplicateValues" dxfId="32" priority="4"/>
+  <conditionalFormatting sqref="A1:A2 A4:A7 A9:A24">
+    <cfRule type="duplicateValues" dxfId="3" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A2 A4:A20">
+  <conditionalFormatting sqref="A1:A2 A4:A7 A9:A20">
+    <cfRule type="duplicateValues" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
+    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3">
     <cfRule type="duplicateValues" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
+  <conditionalFormatting sqref="A8">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
+  <conditionalFormatting sqref="A8">
     <cfRule type="duplicateValues" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2223,21 +2327,21 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.26953125" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.21875" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2258,7 +2362,7 @@
       </c>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44288</v>
       </c>
@@ -2280,10 +2384,10 @@
       </c>
       <c r="H2" s="11">
         <f>COUNT(Tabela147[[#All],[Day]])</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44300</v>
       </c>
@@ -2305,10 +2409,10 @@
       </c>
       <c r="H3" s="12">
         <f>SUM(Tabela147[[#All],[Duration]])</f>
-        <v>0.57291666666666674</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>0.69791666666666674</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44321</v>
       </c>
@@ -2326,7 +2430,7 @@
         <v>0.16319444444444442</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="30">
         <v>44352</v>
       </c>
@@ -2348,21 +2452,29 @@
       </c>
       <c r="H5" s="35"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>44358</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
       <c r="E6" s="3">
         <f>Tabela147[[#This Row],[End Time]]-Tabela147[[#This Row],[Start Time]]</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G6" s="36" t="s">
         <v>34</v>
       </c>
       <c r="H6" s="36"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -2376,7 +2488,7 @@
       </c>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -2386,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -2396,7 +2508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -2406,7 +2518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -2416,7 +2528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -2426,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -2436,7 +2548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -2446,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -2456,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -2466,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -2476,7 +2588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -2486,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -2496,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -2506,7 +2618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -2516,7 +2628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -2526,7 +2638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -2536,7 +2648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2554,13 +2666,13 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A2 A4 A6:A24">
-    <cfRule type="duplicateValues" dxfId="23" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A2 A4 A6:A20">
     <cfRule type="duplicateValues" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="22" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
     <cfRule type="duplicateValues" priority="3"/>
@@ -2577,22 +2689,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB61F12-31A1-4865-A365-EE2C93760A20}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.77734375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2613,7 +2725,7 @@
       </c>
       <c r="H1" s="35"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>44286</v>
       </c>
@@ -2638,7 +2750,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>44321</v>
       </c>
@@ -2663,7 +2775,7 @@
         <v>0.85763888888888895</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>44348</v>
       </c>
@@ -2681,7 +2793,7 @@
         <v>0.45833333333333337</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>44359</v>
       </c>
@@ -2703,7 +2815,7 @@
       </c>
       <c r="H5" s="35"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
@@ -2717,7 +2829,7 @@
       </c>
       <c r="H6" s="36"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
@@ -2731,7 +2843,7 @@
       </c>
       <c r="H7" s="36"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -2741,7 +2853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
@@ -2751,7 +2863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
@@ -2761,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
@@ -2771,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
@@ -2781,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -2791,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -2801,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -2811,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
@@ -2821,7 +2933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
@@ -2831,7 +2943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
@@ -2841,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
@@ -2851,7 +2963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
@@ -2861,7 +2973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
@@ -2871,7 +2983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="4"/>
@@ -2881,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="4"/>
@@ -2891,7 +3003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
       <c r="C24" s="4"/>
@@ -2909,7 +3021,7 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:A24">
-    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A20">
     <cfRule type="duplicateValues" priority="1"/>
@@ -2924,31 +3036,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C227607-00A4-48AA-9A87-27CE805F8079}">
-  <dimension ref="A2:E27"/>
+  <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A25" sqref="A25:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" customWidth="1"/>
-    <col min="2" max="2" width="58.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" customWidth="1"/>
+    <col min="2" max="2" width="58.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="20">
         <f>SUMPRODUCT(Tabela2[QTD], Tabela2[Preço_uni])</f>
-        <v>94.67022</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>97.190219999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -2965,7 +3077,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
@@ -2983,7 +3095,7 @@
         <v>Bluetooth Module HC-05</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>13</v>
       </c>
@@ -3001,7 +3113,7 @@
         <v>IR Emitter and Receiver LED 5mm 940nm</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="25" t="s">
         <v>13</v>
       </c>
@@ -3019,7 +3131,7 @@
         <v>OV7670 Camera Module</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="25" t="s">
         <v>13</v>
       </c>
@@ -3037,7 +3149,7 @@
         <v>TCS3200 Color Sensor</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="27" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="25" t="s">
         <v>13</v>
       </c>
@@ -3055,7 +3167,7 @@
         <v>US-015 Modulo Sensor de Distância Ultrassónico 3.3 - 5V</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>45</v>
       </c>
@@ -3073,7 +3185,7 @@
         <v>Módulo Leitor RFID RC522</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>54</v>
       </c>
@@ -3091,7 +3203,7 @@
         <v>Sensor Sharp 2Y0A21YK</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>52</v>
       </c>
@@ -3109,7 +3221,7 @@
         <v>Ficha Shell ou KK 6 vias 2,54mm</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>52</v>
       </c>
@@ -3127,7 +3239,7 @@
         <v>Terminais para fichas shell ou KK</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
@@ -3145,7 +3257,7 @@
         <v>Cartão RFID Mifare 1k S50 compatível Tag 13,56MHz</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>52</v>
       </c>
@@ -3164,7 +3276,7 @@
         <v>Step-Down para 5V até 8A 40W com 4 Portas USB</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>52</v>
       </c>
@@ -3183,7 +3295,7 @@
         <v>Suporte para 1 pilha 18650 c/ fios</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>52</v>
       </c>
@@ -3202,7 +3314,7 @@
         <v>Interruptor de painel redondo</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>52</v>
       </c>
@@ -3221,7 +3333,7 @@
         <v>Botão de pressão preto redondo para painel</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>52</v>
       </c>
@@ -3240,7 +3352,7 @@
         <v>Carregador 3 Baterias 18650 em série - AC 100~240V DC 12,6V 1A</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>52</v>
       </c>
@@ -3259,7 +3371,7 @@
         <v>Cabo DC 0,2m com conector recto 5,2/2,1 (9,5mm)</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>67</v>
       </c>
@@ -3277,60 +3389,192 @@
         <v>Suporte Fusível Auto/F.Pla &gt;50A</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>67</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="E23" s="8" t="str">
+        <f>HYPERLINK("https://www.alfaelektor.pt/item.php?id=2198",Tabela2[[#This Row],[Produto]])</f>
+        <v>Fusivel 3A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7">
         <v>5.5</v>
       </c>
-      <c r="E23" s="8" t="str">
+      <c r="E24" s="8" t="str">
         <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
         <v>Manga Espiral Wrapping 20-60mm</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8" t="str">
         <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="8">
+        <v>PCB Shield STM32F767ZI</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="E26" s="8" t="str">
         <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="8">
+        <v>Barra (2x8) fêmea 2,54 mm PCB</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="E27" s="8" t="str">
         <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="8">
+        <v>Barra (2x10) fêmea 2,54 mm PCB</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="1">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0.62</v>
+      </c>
+      <c r="E28" s="8" t="str">
+        <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
+        <v>Barra (2x16) fêmea 2,54 mm PCB</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="1">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7">
+        <v>0.69</v>
+      </c>
+      <c r="E29" s="8" t="str">
+        <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
+        <v>Barra (2x17) fêmea 2,54 mm PCB</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="E30" s="8" t="str">
+        <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
+        <v>Barra (2x3) fêmea 2,54 mm PCB</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="E31" s="8" t="str">
+        <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
+        <v>Barra (1x6) fêmea 2,54 mm PCB</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="8">
+        <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8">
+        <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8">
         <f>HYPERLINK(,Tabela2[[#This Row],[Produto]])</f>
         <v>0</v>
       </c>

</xml_diff>